<commit_message>
Better world grid awareness
</commit_message>
<xml_diff>
--- a/planning/flap-calculations.xlsx
+++ b/planning/flap-calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lc\blooDot\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B210C5DC-AC11-411B-9976-073011D91DB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C0A53D-EB93-4A06-AB7C-618B9D3B2689}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{A9394B7E-ABCD-444D-9D89-635D2F5486D8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>koordinate des rechten randes</t>
   </si>
@@ -76,14 +76,28 @@
   </si>
   <si>
     <t>innenstand des linken quadrats lokal</t>
+  </si>
+  <si>
+    <t>left in world</t>
+  </si>
+  <si>
+    <t>gu diff on sheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,10 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,16 +453,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E067665-78E6-4A73-8BAD-2CA6E65A426C}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="11.08984375" customWidth="1"/>
-    <col min="5" max="14" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
+    <col min="6" max="14" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -471,31 +487,31 @@
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>2047</v>
       </c>
       <c r="G3" s="2">
-        <v>2</v>
+        <v>2048</v>
       </c>
       <c r="H3" s="2">
-        <v>3</v>
+        <v>2049</v>
       </c>
       <c r="I3" s="2">
-        <v>4</v>
+        <v>2050</v>
       </c>
       <c r="J3" s="2">
-        <v>5</v>
+        <v>2051</v>
       </c>
       <c r="K3" s="2">
-        <v>6</v>
+        <v>2052</v>
       </c>
       <c r="L3" s="2">
-        <v>7</v>
+        <v>2053</v>
       </c>
       <c r="M3" s="2">
-        <v>8</v>
+        <v>2054</v>
       </c>
       <c r="N3" s="2">
-        <v>9</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -508,39 +524,39 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4:N4" si="0">(CEILING(F5/$C$2,1)-1)*$C$2</f>
-        <v>1274</v>
+        <v>1310701</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>1911</v>
+        <v>1311338</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>2548</v>
+        <v>1311975</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>3185</v>
+        <v>1312612</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="0"/>
-        <v>3822</v>
+        <v>1313249</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="0"/>
-        <v>4459</v>
+        <v>1313886</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="0"/>
-        <v>5096</v>
+        <v>1314523</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" si="0"/>
-        <v>5733</v>
+        <v>1315160</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" si="0"/>
-        <v>6370</v>
+        <v>1315797</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -553,39 +569,39 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5:N5" si="2">$C$1*(F3+1)</f>
-        <v>1280</v>
+        <v>1310720</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="2"/>
-        <v>1920</v>
+        <v>1311360</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="2"/>
-        <v>2560</v>
+        <v>1312000</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>3200</v>
+        <v>1312640</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="2"/>
-        <v>3840</v>
+        <v>1313280</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>4480</v>
+        <v>1313920</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="2"/>
-        <v>5120</v>
+        <v>1314560</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="2"/>
-        <v>5760</v>
+        <v>1315200</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="2"/>
-        <v>6400</v>
+        <v>1315840</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -593,44 +609,44 @@
         <v>9</v>
       </c>
       <c r="E6" s="1">
-        <f>E5-E4</f>
+        <f t="shared" ref="E6:N6" si="3">E5-E4</f>
         <v>3</v>
       </c>
       <c r="F6" s="1">
-        <f>F5-F4</f>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="G6" s="1">
-        <f>G5-G4</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>22</v>
       </c>
       <c r="H6" s="1">
-        <f>H5-H4</f>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>25</v>
       </c>
       <c r="I6" s="1">
-        <f>I5-I4</f>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>28</v>
       </c>
       <c r="J6" s="1">
-        <f>J5-J4</f>
-        <v>18</v>
+        <f t="shared" si="3"/>
+        <v>31</v>
       </c>
       <c r="K6" s="1">
-        <f>K5-K4</f>
-        <v>21</v>
+        <f t="shared" si="3"/>
+        <v>34</v>
       </c>
       <c r="L6" s="1">
-        <f>L5-L4</f>
-        <v>24</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="M6" s="1">
-        <f>M5-M4</f>
-        <v>27</v>
+        <f t="shared" si="3"/>
+        <v>40</v>
       </c>
       <c r="N6" s="1">
-        <f>N5-N4</f>
-        <v>30</v>
+        <f t="shared" si="3"/>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -638,43 +654,43 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ref="E7:N7" si="3">CEILING($C$1/$C$2,1)</f>
+        <f t="shared" ref="E7:N7" si="4">CEILING($C$1/$C$2,1)</f>
         <v>14</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
@@ -683,89 +699,89 @@
         <v>10</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8" si="4">$C$2-E6</f>
+        <f t="shared" ref="E8" si="5">$C$2-E6</f>
         <v>46</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8:N8" si="5">$C$2-F6</f>
-        <v>43</v>
+        <f t="shared" ref="F8:N8" si="6">$C$2-F6</f>
+        <v>30</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="5"/>
-        <v>40</v>
+        <f t="shared" si="6"/>
+        <v>27</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="5"/>
-        <v>37</v>
+        <f t="shared" si="6"/>
+        <v>24</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="5"/>
-        <v>34</v>
+        <f t="shared" si="6"/>
+        <v>21</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="5"/>
-        <v>31</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="5"/>
-        <v>28</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="5"/>
-        <v>25</v>
+        <f t="shared" si="6"/>
+        <v>12</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="5"/>
-        <v>22</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="5"/>
-        <v>19</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="1">
-        <f>E4-$C$2*(E7-1)</f>
-        <v>0</v>
+        <f>(CEILING((E5-$C$1)/$C$2,1)-1)*$C$2</f>
+        <v>-49</v>
       </c>
       <c r="F9" s="1">
-        <f>F4-$C$2*(F7-1)</f>
-        <v>637</v>
+        <f>(CEILING((F5-$C$1)/$C$2,1)-1)*$C$2</f>
+        <v>1310064</v>
       </c>
       <c r="G9" s="1">
-        <f>G4-$C$2*(G7-1)</f>
-        <v>1274</v>
+        <f t="shared" ref="G9:N9" si="7">(CEILING((G5-$C$1)/$C$2,1)-1)*$C$2</f>
+        <v>1310701</v>
       </c>
       <c r="H9" s="1">
-        <f>H4-$C$2*(H7-1)</f>
-        <v>1911</v>
+        <f t="shared" si="7"/>
+        <v>1311338</v>
       </c>
       <c r="I9" s="1">
-        <f>I4-$C$2*(I7-1)</f>
-        <v>2548</v>
+        <f t="shared" si="7"/>
+        <v>1311975</v>
       </c>
       <c r="J9" s="1">
-        <f>J4-$C$2*(J7-1)</f>
-        <v>3185</v>
+        <f t="shared" si="7"/>
+        <v>1312612</v>
       </c>
       <c r="K9" s="1">
-        <f>K4-$C$2*(K7-1)</f>
-        <v>3822</v>
+        <f t="shared" si="7"/>
+        <v>1313249</v>
       </c>
       <c r="L9" s="1">
-        <f>L4-$C$2*(L7-1)</f>
-        <v>4459</v>
+        <f t="shared" si="7"/>
+        <v>1313886</v>
       </c>
       <c r="M9" s="1">
-        <f>M4-$C$2*(M7-1)</f>
-        <v>5096</v>
+        <f t="shared" si="7"/>
+        <v>1314523</v>
       </c>
       <c r="N9" s="1">
-        <f>N4-$C$2*(N7-1)</f>
-        <v>5733</v>
+        <f t="shared" si="7"/>
+        <v>1315160</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -773,44 +789,44 @@
         <v>15</v>
       </c>
       <c r="E10" s="1">
-        <f>E9-(E3*$C$1)</f>
-        <v>0</v>
+        <f t="shared" ref="E10:N10" si="8">E9-(E3*$C$1)</f>
+        <v>-49</v>
       </c>
       <c r="F10" s="1">
-        <f>F9-(F3*$C$1)</f>
-        <v>-3</v>
+        <f t="shared" si="8"/>
+        <v>-16</v>
       </c>
       <c r="G10" s="1">
-        <f>G9-(G3*$C$1)</f>
-        <v>-6</v>
+        <f t="shared" si="8"/>
+        <v>-19</v>
       </c>
       <c r="H10" s="1">
-        <f>H9-(H3*$C$1)</f>
-        <v>-9</v>
+        <f t="shared" si="8"/>
+        <v>-22</v>
       </c>
       <c r="I10" s="1">
-        <f>I9-(I3*$C$1)</f>
-        <v>-12</v>
+        <f t="shared" si="8"/>
+        <v>-25</v>
       </c>
       <c r="J10" s="1">
-        <f>J9-(J3*$C$1)</f>
-        <v>-15</v>
+        <f t="shared" si="8"/>
+        <v>-28</v>
       </c>
       <c r="K10" s="1">
-        <f>K9-(K3*$C$1)</f>
-        <v>-18</v>
+        <f t="shared" si="8"/>
+        <v>-31</v>
       </c>
       <c r="L10" s="1">
-        <f>L9-(L3*$C$1)</f>
-        <v>-21</v>
+        <f t="shared" si="8"/>
+        <v>-34</v>
       </c>
       <c r="M10" s="1">
-        <f>M9-(M3*$C$1)</f>
-        <v>-24</v>
+        <f t="shared" si="8"/>
+        <v>-37</v>
       </c>
       <c r="N10" s="1">
-        <f>N9-(N3*$C$1)</f>
-        <v>-27</v>
+        <f t="shared" si="8"/>
+        <v>-40</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -818,44 +834,44 @@
         <v>16</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:N11" si="6">$C$2+E10</f>
-        <v>49</v>
+        <f t="shared" ref="E11:N11" si="9">$C$2+E10</f>
+        <v>0</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="6"/>
-        <v>46</v>
+        <f t="shared" si="9"/>
+        <v>33</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="6"/>
-        <v>43</v>
+        <f t="shared" si="9"/>
+        <v>30</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="6"/>
-        <v>40</v>
+        <f t="shared" si="9"/>
+        <v>27</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="6"/>
-        <v>37</v>
+        <f t="shared" si="9"/>
+        <v>24</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="6"/>
-        <v>34</v>
+        <f t="shared" si="9"/>
+        <v>21</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="6"/>
-        <v>31</v>
+        <f t="shared" si="9"/>
+        <v>18</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="6"/>
-        <v>28</v>
+        <f t="shared" si="9"/>
+        <v>15</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="6"/>
-        <v>25</v>
+        <f t="shared" si="9"/>
+        <v>12</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="6"/>
-        <v>22</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -863,327 +879,405 @@
         <v>11</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" ref="E12" si="7">$C$1+E8-E10</f>
+        <f t="shared" ref="E12" si="10">$C$1+E8-E10</f>
+        <v>735</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" ref="F12:N12" si="11">$C$1+F8-F10</f>
         <v>686</v>
       </c>
-      <c r="F12" s="1">
-        <f t="shared" ref="F12:N12" si="8">$C$1+F8-F10</f>
+      <c r="G12" s="1">
+        <f t="shared" si="11"/>
         <v>686</v>
       </c>
-      <c r="G12" s="1">
-        <f t="shared" si="8"/>
+      <c r="H12" s="1">
+        <f t="shared" si="11"/>
         <v>686</v>
       </c>
-      <c r="H12" s="1">
-        <f t="shared" si="8"/>
+      <c r="I12" s="1">
+        <f t="shared" si="11"/>
         <v>686</v>
       </c>
-      <c r="I12" s="1">
-        <f t="shared" si="8"/>
+      <c r="J12" s="1">
+        <f t="shared" si="11"/>
         <v>686</v>
       </c>
-      <c r="J12" s="1">
-        <f t="shared" si="8"/>
+      <c r="K12" s="1">
+        <f t="shared" si="11"/>
         <v>686</v>
       </c>
-      <c r="K12" s="1">
-        <f t="shared" si="8"/>
+      <c r="L12" s="1">
+        <f t="shared" si="11"/>
         <v>686</v>
       </c>
-      <c r="L12" s="1">
-        <f t="shared" si="8"/>
+      <c r="M12" s="1">
+        <f t="shared" si="11"/>
         <v>686</v>
       </c>
-      <c r="M12" s="1">
-        <f t="shared" si="8"/>
+      <c r="N12" s="1">
+        <f t="shared" si="11"/>
         <v>686</v>
       </c>
-      <c r="N12" s="1">
-        <f t="shared" si="8"/>
-        <v>686</v>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="1">
+        <f>CEILING((F9-$C$1*$F3)/$C$2-F7/2,1)</f>
+        <v>-7</v>
+      </c>
+      <c r="G13" s="1">
+        <f>CEILING((G9-$C$1*$F3)/$C$2-G7/2,1)</f>
+        <v>6</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" ref="G13:N13" si="12">CEILING((H9-$C$1*$F3)/$C$2-H7/2,1)</f>
+        <v>19</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="12"/>
+        <v>32</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="12"/>
+        <v>45</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="12"/>
+        <v>58</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="12"/>
+        <v>71</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="12"/>
+        <v>84</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="12"/>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="1">
+        <f>G13-F13</f>
         <v>13</v>
       </c>
-      <c r="E14" s="1">
-        <f>E11-E10</f>
-        <v>49</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" ref="F14:N14" si="9">F11-F10</f>
-        <v>49</v>
-      </c>
-      <c r="G14" s="1">
-        <f t="shared" si="9"/>
-        <v>49</v>
-      </c>
       <c r="H14" s="1">
-        <f t="shared" si="9"/>
-        <v>49</v>
+        <f t="shared" ref="H14:N14" si="13">H13-G13</f>
+        <v>13</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="9"/>
-        <v>49</v>
+        <f t="shared" si="13"/>
+        <v>13</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="9"/>
-        <v>49</v>
+        <f t="shared" si="13"/>
+        <v>13</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="9"/>
-        <v>49</v>
+        <f t="shared" si="13"/>
+        <v>13</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="9"/>
-        <v>49</v>
+        <f t="shared" si="13"/>
+        <v>13</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="9"/>
-        <v>49</v>
+        <f t="shared" si="13"/>
+        <v>13</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="9"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="1">
-        <f>E6+E8</f>
-        <v>49</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" ref="F15:N15" si="10">F6+F8</f>
-        <v>49</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="10"/>
-        <v>49</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" si="10"/>
-        <v>49</v>
-      </c>
-      <c r="I15" s="1">
-        <f t="shared" si="10"/>
-        <v>49</v>
-      </c>
-      <c r="J15" s="1">
-        <f t="shared" si="10"/>
-        <v>49</v>
-      </c>
-      <c r="K15" s="1">
-        <f t="shared" si="10"/>
-        <v>49</v>
-      </c>
-      <c r="L15" s="1">
-        <f t="shared" si="10"/>
-        <v>49</v>
-      </c>
-      <c r="M15" s="1">
-        <f t="shared" si="10"/>
-        <v>49</v>
-      </c>
-      <c r="N15" s="1">
-        <f t="shared" si="10"/>
-        <v>49</v>
+        <f t="shared" si="13"/>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1">
+        <f>E11-E10</f>
+        <v>49</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" ref="F16:N16" si="14">F11-F10</f>
+        <v>49</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="1">
+        <f>E6+E8</f>
+        <v>49</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" ref="F17:N17" si="15">F6+F8</f>
+        <v>49</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E18" s="1">
         <f>E6</f>
         <v>3</v>
       </c>
-      <c r="F16" s="1">
-        <f t="shared" ref="F16:N16" si="11">F6</f>
-        <v>6</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" si="11"/>
-        <v>9</v>
-      </c>
-      <c r="H16" s="1">
-        <f t="shared" si="11"/>
-        <v>12</v>
-      </c>
-      <c r="I16" s="1">
-        <f t="shared" si="11"/>
-        <v>15</v>
-      </c>
-      <c r="J16" s="1">
-        <f t="shared" si="11"/>
-        <v>18</v>
-      </c>
-      <c r="K16" s="1">
-        <f t="shared" si="11"/>
-        <v>21</v>
-      </c>
-      <c r="L16" s="1">
-        <f t="shared" si="11"/>
-        <v>24</v>
-      </c>
-      <c r="M16" s="1">
-        <f t="shared" si="11"/>
-        <v>27</v>
-      </c>
-      <c r="N16" s="1">
-        <f t="shared" si="11"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="1">
-        <f>E11</f>
-        <v>49</v>
-      </c>
-      <c r="F17" s="1">
-        <f t="shared" ref="F17:N17" si="12">F11</f>
-        <v>46</v>
-      </c>
-      <c r="G17" s="1">
-        <f t="shared" si="12"/>
+      <c r="F18" s="1">
+        <f t="shared" ref="F18:N18" si="16">F6</f>
+        <v>19</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="16"/>
+        <v>22</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="16"/>
+        <v>25</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="16"/>
+        <v>28</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="16"/>
+        <v>31</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="16"/>
+        <v>34</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="16"/>
+        <v>37</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="16"/>
+        <v>40</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="16"/>
         <v>43</v>
-      </c>
-      <c r="H17" s="1">
-        <f t="shared" si="12"/>
-        <v>40</v>
-      </c>
-      <c r="I17" s="1">
-        <f t="shared" si="12"/>
-        <v>37</v>
-      </c>
-      <c r="J17" s="1">
-        <f t="shared" si="12"/>
-        <v>34</v>
-      </c>
-      <c r="K17" s="1">
-        <f t="shared" si="12"/>
-        <v>31</v>
-      </c>
-      <c r="L17" s="1">
-        <f t="shared" si="12"/>
-        <v>28</v>
-      </c>
-      <c r="M17" s="1">
-        <f t="shared" si="12"/>
-        <v>25</v>
-      </c>
-      <c r="N17" s="1">
-        <f t="shared" si="12"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="1">
-        <f>E16+E17</f>
-        <v>52</v>
-      </c>
-      <c r="F18" s="1">
-        <f t="shared" ref="F18:N18" si="13">F16+F17</f>
-        <v>52</v>
-      </c>
-      <c r="G18" s="1">
-        <f t="shared" si="13"/>
-        <v>52</v>
-      </c>
-      <c r="H18" s="1">
-        <f t="shared" si="13"/>
-        <v>52</v>
-      </c>
-      <c r="I18" s="1">
-        <f t="shared" si="13"/>
-        <v>52</v>
-      </c>
-      <c r="J18" s="1">
-        <f t="shared" si="13"/>
-        <v>52</v>
-      </c>
-      <c r="K18" s="1">
-        <f t="shared" si="13"/>
-        <v>52</v>
-      </c>
-      <c r="L18" s="1">
-        <f t="shared" si="13"/>
-        <v>52</v>
-      </c>
-      <c r="M18" s="1">
-        <f t="shared" si="13"/>
-        <v>52</v>
-      </c>
-      <c r="N18" s="1">
-        <f t="shared" si="13"/>
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="1">
+        <f>E11</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" ref="F19:N19" si="17">F11</f>
+        <v>33</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="17"/>
+        <v>27</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="17"/>
+        <v>24</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="17"/>
+        <v>21</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="17"/>
+        <v>18</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="17"/>
+        <v>15</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="1">
+        <f>E18+E19</f>
+        <v>3</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" ref="F20:N20" si="18">F18+F19</f>
+        <v>52</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="18"/>
+        <v>52</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="18"/>
+        <v>52</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="18"/>
+        <v>52</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="18"/>
+        <v>52</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="18"/>
+        <v>52</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="18"/>
+        <v>52</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="18"/>
+        <v>52</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="18"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="1">
-        <f>D16+E17</f>
-        <v>49</v>
-      </c>
-      <c r="F19" s="1">
-        <f>E16+F17</f>
-        <v>49</v>
-      </c>
-      <c r="G19" s="1">
-        <f t="shared" ref="G19:N19" si="14">F16+G17</f>
-        <v>49</v>
-      </c>
-      <c r="H19" s="1">
-        <f t="shared" si="14"/>
-        <v>49</v>
-      </c>
-      <c r="I19" s="1">
-        <f t="shared" si="14"/>
-        <v>49</v>
-      </c>
-      <c r="J19" s="1">
-        <f t="shared" si="14"/>
-        <v>49</v>
-      </c>
-      <c r="K19" s="1">
-        <f t="shared" si="14"/>
-        <v>49</v>
-      </c>
-      <c r="L19" s="1">
-        <f t="shared" si="14"/>
-        <v>49</v>
-      </c>
-      <c r="M19" s="1">
-        <f t="shared" si="14"/>
-        <v>49</v>
-      </c>
-      <c r="N19" s="1">
-        <f t="shared" si="14"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
+      <c r="E21" s="1">
+        <f>D18+E19</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E18+F19</f>
+        <v>36</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" ref="G21:N21" si="19">F18+G19</f>
+        <v>49</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="19"/>
+        <v>49</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="19"/>
+        <v>49</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="19"/>
+        <v>49</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="19"/>
+        <v>49</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="19"/>
+        <v>49</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="19"/>
+        <v>49</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="19"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>